<commit_message>
GenreSelectBefore view filter 수정
</commit_message>
<xml_diff>
--- a/movies1.xlsx
+++ b/movies1.xlsx
@@ -356,84 +356,84 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>프리스트</t>
+          <t>나는 악마를 사랑했다</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>흡혈귀 떼를 물리치는 전사가 된 신부. 신부로 분한 폴 베터니가 납치된 조카를 구출하기 위해 사활을 건 싸움을 시작한다.</t>
+          <t>다정하고 똑똑한 그가 잔혹한 연쇄 살인마라니! 테드 번디와 사랑에 빠진 싱글 맘 리즈는 그의 범죄 사실을 수년간 믿지 못한다. 악명 높은 범죄 실화를 바탕으로 한 영화.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1시간 27분</t>
+          <t>1시간 50분</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2011</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>만 15세 이상의 자가 관람할 수 있는 영화</t>
+          <t>청소년은 관람할 수 없는 영화</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/jsgGe9NCko3c-j0wGZ7FSwVlHs0/AAAABVPNGsRv_baoIhpbf9OIYFQNEoRzJu0ekFZtBel_Z7QYiBs601vgdHTlaN80iK4v8t-Pg4mV6kmY35i2MKOHuatVzDUndhK2kxvlzzk.png?r=985</t>
+          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/jsgGe9NCko3c-j0wGZ7FSwVlHs0/AAAABdm0zRt2Ht2uRe55sWJ3YdedjRo-gT5fT_-Y4o54WdyYuiBhdwqXC12CQ8dvs2BwPzhA2U4-_5oVTiP93bPxLYLNU-zlINlKRVc3TOZXtRabsQ3Jty9U1cCcsyL39fvHgOGHFFP-HxEx4T6rTJEpIT6auz33FaaAQYOO576Hdgw.png?r=43e</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>스콧 스튜어트</t>
+          <t>조 벌린저</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>폴 베타니,칼 어번,캠 지간데이,매기 큐,릴리 콜린스,브래드 듀리프,스티븐 모이어,크리스토퍼 플러머,앨런 데일,메이천 에이믹</t>
+          <t>잭 에프론,릴리 콜린스,카야 스코델라리오,제프리 도너번,앤절라 서라피언,짐 파슨스,존 말코비치,헤일리 조엘 오즈먼트,딜란 베이커,브라이언 게러티</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>코리 굿맨</t>
+          <t>마이클 워위</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>미국 영화,액션 &amp; 어드벤처,SF &amp; 판타지,액션·SF &amp; 판타지</t>
+          <t>영화·실화 바탕,전기 영화,미국 영화,드라마 장르 영화</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>무서운</t>
+          <t>불길한 영화,어두운 분위기</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/E8vDc_W8CLv7-yMQu8KMEC7Rrr8/AAAABV8IPWOpOPwvXBmiqL6yD1ZW538lYX9_oABbGPx5IPVt61gzu2erxLrfU68e1yHpptdq8hEL1OIMktdeXPzfAbJqs8dheAzeEQ.jpg?r=d15</t>
+          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/E8vDc_W8CLv7-yMQu8KMEC7Rrr8/AAAABYT0jbuE5pN52ej9OKRN7gYZiFyjoi5-di_zVHXR8dG5qCmEZBWfwz3PBePIlEHGrdNk7G0vDkyH_2meZfOC415JL_QhPVpeQg.jpg?r=bf5</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>레지던트 이블 5: 최후의 심판</t>
+          <t>비포미드나잇</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>모든 게 끝난 줄 알았다. 하지만 눈을 떠보니 세상은 끔찍한 돌연변이 천지. 엄브렐라 사의 치명적인 T-바이러스로 인해 사람들이 언데드 군단으로 변해 버린 상황. 멸종 위기에 처한 인류에게 남은 희망이 있다면, 그것은 앨리스뿐.</t>
+          <t>파리에서의 재회 후, 어엿한 가정을 꾸린 제시와 셀린. 두 딸을 기르며 행복한 삶을 살지만, 뭔가를 잃어버린 듯한 느낌을 지울 수 없다. 바래 버린 로맨스를 되찾기 위한 두 사람의 여행. 《비포 선라이즈》, 그 두 번째 이야기.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1시간 35분</t>
+          <t>1시간 48분</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2012</t>
+          <t>2013</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -443,117 +443,117 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/jsgGe9NCko3c-j0wGZ7FSwVlHs0/AAAABRTRYK1UH0kEAHq2qkpMOgIojnqUwi8ogYq8xYR6EZruQWV2orGjlyCJbEBS0LS8ZiDAm2pdFn7kxthBtNA8PenY-7sBvWCYGd7rWTM.png?r=a23</t>
+          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/jsgGe9NCko3c-j0wGZ7FSwVlHs0/AAAABVT0I6CMDe7rfwOqqvBqExzwU10puP7LWLDnMot_aZUjsTu5dfGIaWva4omQDekba_YCz0HPK4SNWxU3wGy4mtD2sD7q9Aie18CLoZM.png?r=aa4</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>폴 앤더슨</t>
+          <t>리처드 링클레이터</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>밀라 요보비치,시에나 길로리,미셸 로드리게즈,Aryana Engineer,리빙빙,보리스 코조,조핸 어브,Robin Kasyanov,케빈 두런드,Ofilio Portillo,오데드 페르,콜린 살몬</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr"/>
+          <t>에단 호크,줄리 델피,샤뮤스 데이비 핏츠패트릭,제니퍼 프라이어,샬럿 프라이어,크세니아 칼로예로풀루,월터 라살리,아리안 라베드,야니스 파파도풀로스,아티나 라힐 창가리,파노스 코로니스</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>리처드 링클레이터,줄리 델피,에단 호크</t>
+        </is>
+      </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>미국 영화,액션 &amp; 어드벤처,액션·스릴러,SF &amp; 판타지</t>
+          <t>미국 영화,드라마 장르 영화,드라마 장르 영화·로맨스,영화·로맨스</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>폭력,흥미진진</t>
+          <t>로맨스</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/E8vDc_W8CLv7-yMQu8KMEC7Rrr8/AAAABd8L9QqfCT-H0vmeHclTTh4AAsuiHhdyyzIqjhLAQdR5q-qE0xK_VEFR-3e3KCtAw9tlwK5kokTqqypOVzKjeHW82qEtbFcjcQ.jpg?r=a90</t>
+          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/E8vDc_W8CLv7-yMQu8KMEC7Rrr8/AAAABZ2paG6b8Cz9INGHJeOlme--pjwGVUSNYQUxUdG9HdLJNeDovHxPqSBf_3SYxCpfcoh-d7ry6NymZHzBBD6tkkzZmv3jxBJcgQ.jpg?r=539</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>무서운 영화4</t>
+          <t>산호초를 따라서</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>폭소의 도가니 《무서운 영화》가 네 번째 이야기로 돌아왔다! 코미디 황금 명맥을 이어 온 패러디 영화의 진수. 《밀리언 달러 베이비》 《쏘우》 《브로크백 마운틴》까지, 주옥같은 영화의 명장면을 한데 모았다. 배꼽 붙들어 매시길.</t>
+          <t>죽어가는 산호초를 기록하는 사람들. 전 세계의 다이버와 과학자, 포토그래퍼들이 모여 거대한 수중 캠페인을 만들어간다. 생명의 바다를 지키기 위해.</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1시간 23분</t>
+          <t>1시간 29분</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2006</t>
+          <t>2017</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>만 15세 이상의 자가 관람할 수 있는 영화</t>
+          <t>만 12세 이상의 자가 관람할 수 있는 영화</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/jsgGe9NCko3c-j0wGZ7FSwVlHs0/AAAABYkHBOURChm1ZcloE34OEpOMWn2h8715bba4V9PDrs2Lq0akxccwgRZXk5wRyWOXpI_JEPaiobH0h61wlImwvdDvEVstvW7Ca3a084w.png?r=c58</t>
+          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/jsgGe9NCko3c-j0wGZ7FSwVlHs0/AAAABQc8k7srNoyW2WqnLh6y3RdW1q2iQFEjljYwbwIN95FqvArdTx7UyfuLE12q6B4571GyNJ0d-GrsLtb_r3CQ6DfrFxKO9Hngxu1WEcbHh_TIzkNYSYTGss7Vc_yPcZTwlg7jOMDh2SpIZQ097TSJvQD1KGQLcJ8c1XfcboqpSDU.png?r=059</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>데이비드 주커</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>안나 페리스,레지나 홀,크레이그 비에코,빌 풀먼,앤서니 앤더슨,레슬리 닐슨,몰리 샤논,마이클 마센,크리스 엘리엇,카르멘 일렉트라,크리스 엘리엇,샤킬 오닐</t>
-        </is>
-      </c>
+          <t>제프 올로프스키</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr">
         <is>
-          <t>크레이그 메이진,짐 아브라함,팻 프로프트</t>
+          <t>데이비스 쿰,비키 커티스,제프 올로프스키</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>미국 영화,영화·호러,공포 코미디 영화,코미디</t>
+          <t>미국 영화,다큐멘터리,과학&amp;자연 다큐멘터리</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>선정적,푼수 캐릭터</t>
+          <t>논쟁을 부르는</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/E8vDc_W8CLv7-yMQu8KMEC7Rrr8/AAAABaZ5LnJHsWfaqDtadYdMMCklcO-89WwwS-C_TNDMsXQeEmxGAk8tGuFmf6_jzK8_NmTR978pdMn5EoT71iavVURBY48mXVkktQ.jpg?r=a7e</t>
+          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/E8vDc_W8CLv7-yMQu8KMEC7Rrr8/AAAABQ8Ej8eI55aAjxTz7iG1CJ18Zdm4KCysWLlSJScXLtxB75-CTXaeGy3lhGPlmeen9i8HuI5ir-bYIzBjyAc7pd8Du0AVHYG1og.jpg?r=8a5</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>인시디어스 3</t>
+          <t>우산 혁명: 소년 vs. 제국</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>죽은 엄마와 얘기하고 싶어 영매 엘리스를 찾아간 소녀 퀸. 그날 이후, 퀸에게 이상한 일들이 일어나기 시작한다. 환영인지 실재인지 모를 남자의 출몰, 알 수 없는 말을 건네는 이웃 할머니. 퀸을 위협하는 존재의 실체는 과연 무엇인가.</t>
+          <t>10대 학생운동가 조슈아 웡이 이끄는 홍콩의 젊은 시민들. 성난 그들이 거리로 나섰다. 오직 조국 홍콩의 자치를 수호하기 위해.</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1시간 37분</t>
+          <t>1시간 18분</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2015</t>
+          <t>2017</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -563,601 +563,557 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/jsgGe9NCko3c-j0wGZ7FSwVlHs0/AAAABW8_qV_Sd28ttKNcJ6c40dTz0oZ2RNJv4on4E8kigoO2n5m3iPsRZ8ZtBIqwzYmuvygPzeIqx3pIxA4pvzQ3O0bF_umZ5ldrmNkz2Sg.png?r=6d1</t>
+          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/jsgGe9NCko3c-j0wGZ7FSwVlHs0/AAAABc6xPhYkutDryEdQ-IlItXJ8KA5WyWp31KJXUB-JyjmhXbRhVZBO86E0l9ZbDbJdvS95ToGy2xg85lqJXpoiKlLdldXCmUfMTzWxJ07tmZhfiJgxdKaIqyg6CFCDu01bDdCeo6_VhY7hmnDSVdBrB4wdUpfzYt2UXt_ryjf6zY4.png?r=72c</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>리 워넬</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>더모트 멀로니,스테퍼니 스콧,린 샤예,앵거스 샘슨,리 워넬,테이트 바니,마이클 리드 매케이,스티브 콜터,헤일리 키요코,코벳 턱</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>리 워넬</t>
-        </is>
-      </c>
+          <t>조 피스카텔라</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr">
         <is>
-          <t>미국 영화,영화·호러,비명 유발·10대</t>
+          <t>전기 영화,미국 영화,십대 영화,다큐멘터리</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>등골 서늘,무서운</t>
+          <t>감동</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/E8vDc_W8CLv7-yMQu8KMEC7Rrr8/AAAABWeuZ6UXz8kepcR5hBIAZN7F3px1IIfQjadgmaCC6bCLVSuLCUnYBRRnwsYXle4EaDE2jWsdQNuYl0G0WbRnJUSPTU29t9QG0w.jpg?r=86c</t>
+          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/E8vDc_W8CLv7-yMQu8KMEC7Rrr8/AAAABer-NIWUJs5I-g9Io9m9WYfL-pV9pGW1UAtbHjeX00IJ9lBpEmYic2EG34N9hEQlFfHErNcQGuMmnKZlD1tBQIICS8q_cKWMRg.jpg?r=0f5</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>직쏘</t>
+          <t>길버트 그레이프</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>잔혹하게 살해당한 시신이 차례로 발견됐다. 10년 전 세상을 뒤흔들었던 직쏘 킬러를 모방한 사건이라 여겼다. 하지만 희생자 부검 결과 이미 죽은 직쏘의 혈흔이 발견되는데! 그렇게, 게임이 다시 시작됐다.</t>
+          <t>몇 년째 가장 역할을 떠맡아 온 길버트. 지적장애 동생 등 돌봐야 할 가족 때문에 어깨가 무겁다. 어느 날, 출구 없는 삶에 한 여자가 나타나는데. 인생의 희망도 찾아오려나.</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1시간 31분</t>
+          <t>1시간 57분</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2017</t>
+          <t>1993</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>청소년은 관람할 수 없는 영화</t>
+          <t>만 12세 이상의 자가 관람할 수 있는 영화</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/jsgGe9NCko3c-j0wGZ7FSwVlHs0/AAAABehsP1MePrV0tht3iMCEOGodGbPc8cNbX7Vxpfvj9aSAxu_jP3cxBqLeKlqy0rpRTlm8b_rrEvFoRVH4uSJeNIsu9NL-HMPIB2Gqu3k.png?r=d2f</t>
+          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/jsgGe9NCko3c-j0wGZ7FSwVlHs0/AAAABco-VarQhubfq4aYQ3H8jYkRw9EeV6TH4mCCSHZm-018WMlWPbA6ZAwFFvG59k6JyxOWEbaAcIi3pnuNeJxSj9EU5m9eRZBmxmjDrBg.png?r=2e8</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>스피리그 형제</t>
+          <t>라세 할스트롬</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>맷 패스모어,토빈 벨,칼럼 키스 레니,해나 에밀리 앤더슨,클레 베넷,로라 밴더보트,폴 브론스틴,만델라 밴 피블스,브리트니 앨런,조사이아 블랙</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>조시 스톨버그,피트 골드핑거</t>
-        </is>
-      </c>
+          <t>조니 뎁,레오나르도 디카프리오,줄리엣 루이스,메리 스틴버겐,달린 케이츠,로라 해링턴,메리 케이트 셸하트,케빈 타이,존 C. 라일리,크리스핀 글로버</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr">
         <is>
-          <t>미국 영화,영화·호러,피투성이 호러 영화,영화·슬래셔 &amp; 연쇄살인범</t>
+          <t>미국 영화,영화·도서 원작,드라마 장르 영화,드라마 장르 영화·로맨스</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>무서운,폭력</t>
+          <t>색다른 이야기,가슴 뭉클</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/E8vDc_W8CLv7-yMQu8KMEC7Rrr8/AAAABapEP48FAagJjYZPiErcELfXN5J09GSzd89YernWsCn8QIam-gGCTlaxYkfOqXnayrLXQdsfIEPCGGUvoU3f0BJ_dt3jo380UA.jpg?r=059</t>
+          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/E8vDc_W8CLv7-yMQu8KMEC7Rrr8/AAAABQheMiPwyOdivZdnz2Qtb8RxTXmADzldm-zJC8ARi9kWNASAo63-he2g8yDwqNw6M7mi3NJU3ws9o8gGTO-4v28SgdsJ-NMg2w.jpg?r=f44</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>제인 도</t>
+          <t>나우이즈굿</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>가업으로 부검 일을 함께하는 아버지와 아들. 어느 날 밤, 신원 미상의 여자 시체 한 구를 맡게 되는데. 시체에서 발견되는 끔찍한 흔적, 그 설명할 수 없는 사인은 무엇인가.</t>
+          <t>암과의 싸움에서 패색이 완연해졌음을 알고 있는 10대 소녀는 남은 일생을 마음껏 즐기기로 결심하고 격정적인 연애까지 시작한다.</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1시간 26분</t>
+          <t>1시간 42분</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>2012</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>청소년은 관람할 수 없는 영화</t>
+          <t>만 15세 이상의 자가 관람할 수 있는 영화</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/jsgGe9NCko3c-j0wGZ7FSwVlHs0/AAAABa9hsOxm2kiNlOAWDiRLAkOYb8x395BhMlL7bv9Zz-6KL10riMj4rci-uFd_3pICvLts3Kx223ebz71K1dIDSut1V76gDw5hCgGrR80.png?r=e98</t>
+          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/jsgGe9NCko3c-j0wGZ7FSwVlHs0/AAAABVJ8KQtejVrODVuGLNeuIWWUYjHdL27ghQe1Ws38ymC4e5tk0MrIXfzJToboqWqdH_XsOi7be5qj3w0LJnVoOKy69zjaTrAJOdpNexo.png?r=f62</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>안드레 외브레달</t>
+          <t>올 파커</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>에밀 허시,브라이언 콕스,오펠리아 로비본드,마이클 맥엘하튼,파커 소여스,제인 페리,올웬 캐서린 켈리</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>이언 골드버그,리처드 나잉</t>
-        </is>
-      </c>
+          <t>다코타 패닝,제러미 어바인,패디 콘시딘,올리비아 윌리암스,카야 스코델라리오,에드가 캐넘,조 콜,줄리아 포드,줄리언 워덤,조세프 알틴</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr">
         <is>
-          <t>미국 영화,미스터리,영화·호러,피투성이 호러 영화</t>
+          <t>십대 영화,십대 로맨스,영화·도서 원작,영국 영화</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>불길한 영화,무서운</t>
+          <t>가슴 뭉클,감정 풍부</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/E8vDc_W8CLv7-yMQu8KMEC7Rrr8/AAAABeni972qYGnAQfz_bCszDMmddGgP1H0ODiJ5udFo8LvC_EUgQCDf1toWxcFrR_NsuuHIoLH9g7HRV8F0njUEYFZJPVK9p1DEZA.jpg?r=bed</t>
+          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/E8vDc_W8CLv7-yMQu8KMEC7Rrr8/AAAABbVjnCDe0sUvYS63yHGhziq94XqayIw_Jvh7tYfbCSZLq2lgdOJgTTM1jiP7mKgsWJ-1OuY35YBA0oegHaYj082fLJqbzeLd1g.jpg?r=2e3</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>슬렌더 맨</t>
+          <t>6년의 사랑</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>친구가 사라졌다! 인터넷 괴담 속 존재 슬렌더맨을 소환하는 의식을 치른 뒤 일어난 일. 그리고 실종된 친구를 찾기 위해 또다시 그를 부르고 말았으니. 절대로 눈을 떠선 안 돼! 눈을 마주치면 미치거나 끔찍한 죽음을 맞게 될 테니.</t>
+          <t>6년을 함께 한 열정적인 커플에게 대학 졸업을 앞두고 예상치 못한 취업 기회가 생기면서 이들의 미래는 불투명해지기 시작한다.</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1시간 33분</t>
+          <t>1시간 19분</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2018</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>만 15세 이상의 자가 관람할 수 있는 영화</t>
+          <t>청소년은 관람할 수 없는 영화</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/jsgGe9NCko3c-j0wGZ7FSwVlHs0/AAAABe5eaazSYRimea-UIj75h8T3BfhPi2ymuTxvs6BRC4ke9HABfnHLepqmETAbVD2FGExxFgNjK6Ye1RRHLs0zV1d2hIQIb3W6RLz3haw.png?r=eb8</t>
+          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/jsgGe9NCko3c-j0wGZ7FSwVlHs0/AAAABTwEe1utLKpVB8SooZu762h-_4xE8VzTabheRvcLCyLi7UDZs3BTcTjiG_cGhkAWOgf-QD29ZcBWiW15t_32tm2Yy9heGOvdFp6JpOw.png?r=170</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>실뱅 화이트</t>
+          <t>한나 피델</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>조이 킹,줄리아 골다니 텔레스,재즈 싱클레어,애너리즈 바쏘,앨릭스 피츠앨런,테일러 리처드슨,하비에르 보테트,제시카 블랭크,마이클 라일리 버크,케빈 채프먼</t>
+          <t>타이사 파미가,벤 로젠필드,린지 버지,조슈아 레오나드,제니퍼 라플러,피터 백,다나 휠러 니콜슨,제이슨 뉴먼,몰리 맥마이클</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>데이비드 버크</t>
+          <t>한나 피델</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>미국 영화,영화·호러,영화·호러·초자연,비명 유발·10대</t>
+          <t>미국 영화,드라마 장르 영화,드라마 장르 영화·로맨스,드라마 장르 영화·관능적</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>등골 서늘,무서운</t>
+          <t>관능적,감정 풍부</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/E8vDc_W8CLv7-yMQu8KMEC7Rrr8/AAAABUTbv2TBnLkNScM6as41VeOdQIBC1EYZXZYwN3XjmhEsAjqOFMhrQ_YoOHJbvIjBy6SHeHUjFvVGY4ftn0Xiq0SodYd2D8ooYQ.jpg?r=544</t>
+          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/E8vDc_W8CLv7-yMQu8KMEC7Rrr8/AAAABcHcD2eQNU5o30T6zH63YW0-d5aF4lGU8-0aqhHdzOelP7CDg0mhcp42oZdWxG0NF2fJ7PonXACS_3IgxC2Fe85A5wtA4JUXQw.jpg?r=c99</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>웜바디스</t>
+          <t>디스커버리</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>젊은 남자의 뇌를 먹고 그 안의 기억을 흡수하게 된 신생 좀비가 그 남자의 여자친구와 사랑에 빠진다.</t>
+          <t>하버 박사가 사후세계의 존재를 증명한 '디스커버리' 후 자살이 폭증한다. 박사는 위험한 실험에 매달리고, 그를 불신하는 아들 윌은 위기의 여인 아일라와 가까워진다.</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1시간 37분</t>
+          <t>1시간 42분</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2013</t>
+          <t>2017</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>만 15세 이상의 자가 관람할 수 있는 영화</t>
+          <t>청소년은 관람할 수 없는 영화</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/jsgGe9NCko3c-j0wGZ7FSwVlHs0/AAAABeET1yHYPGFvitGkiPtwld8rNp355QpAtkvtinV6pqNY_g89RSldGc14nVicfTizB27zIwDX08C7SbWHG2Kcis4E1LQy_ZSTyBs5rWQ.png?r=48a</t>
+          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/jsgGe9NCko3c-j0wGZ7FSwVlHs0/AAAABUknS39uA7jBr-pyVLyrlnPoKtkXDwnfQjpLy-JSrx3me7cDLi9CcRkMOMD4J2SiPxJLoB_lz5PorUdzL0UJqxRkBlQEmTbcLj0_vFb8nhPDnDSJ6xSLGhmz5-E_zXs4GbmsTuHC5HbQrkwGIVJCkrNVyuQ7XRuuo3QNlDir1Uc.png?r=97d</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>조너선 러빈</t>
+          <t>찰리 맥다월</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>니컬러스 홀트,테레사 팔머,애널리 팁튼,롭 코드리,데이브 프랭코,존 말코비치,코리 하드릭트,대니얼 린드레스케이,뱅상 르클레르크,클리퍼드 러듀크베일런코트</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr"/>
+          <t>제이슨 시걸,루니 마라,로버트 레드퍼드,라일리 키오,제시 플리먼스,론 캐나다</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>찰리 맥다월,저스틴 레이더</t>
+        </is>
+      </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>미국 영화,영화·도서 원작,영화·호러,공포 코미디 영화</t>
+          <t>미국 영화,SF &amp; 판타지,SF 영화·드라마 장르,미스터리</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>무서운,로맨스</t>
+          <t>현실 붕괴,잔잔한 분위기</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/E8vDc_W8CLv7-yMQu8KMEC7Rrr8/AAAABfLvspMQtNe6AAUi6xufy2J8hafX-zYAk0uVPEXwFV_yKnGKJtwlpmjkTGd36vcFF8h7qOcm6rDMdE1_y-8-SfD-8yXr1OJ66w.jpg?r=902</t>
+          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/E8vDc_W8CLv7-yMQu8KMEC7Rrr8/AAAABa3gJ7KzqdTiKpL5MteOrm7s7O0FhI5htNLgqmEskZi3reTevX7j87FLqM-YQmLYFSHJfNJF4uQ6ycouxZcmM4H16_pGYqt_tw.jpg?r=2be</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>파이널 데스티네이션 5</t>
+          <t>오직 사랑하는 이들만이 살아남는다</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>끔찍한 다리 붕괴 사고에서 가까스로 목숨을 건진 사람들. 생존의 기쁨도 잠시, 다시 죽음의 그림자가 드리운다. 사신과의 싸움을 시작한 그들. 달라진 죽음의 규칙을 발견해 잔혹한 운명을 바꿀 수 있을는지. 당신, 아직도 살아있는가?</t>
+          <t>지구 반대편에 사는 뱀파이어 부부. 몸은 떨어져 있어도 마음만은 함께다. 남편의 우울한 목소리에 아내가 달려오면서 둘은 재회하지만 기쁨도 잠시, 철없는 처제의 등장으로 곤경에 빠지고 만다. 고이 잠재워둔 뱀파이어 본능까지 눈을 뜨고.</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>1시간 31분</t>
+          <t>2시간 3분</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2011</t>
+          <t>2013</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>청소년은 관람할 수 없는 영화</t>
+          <t>만 15세 이상의 자가 관람할 수 있는 영화</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/jsgGe9NCko3c-j0wGZ7FSwVlHs0/AAAABR3-UfHWT9bfciEGijC3xsw4orvarbM5ey74aXLDRmwYn2O-zgmsS8HpqBs5TxOcSW_f3kF3a_AZiDeCFbUdZpFI7t-pQisak-AJOTA.png?r=931</t>
+          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/jsgGe9NCko3c-j0wGZ7FSwVlHs0/AAAABbzJPi1hGY-3uEJtQ6Zs8jO57HNBG6FYJlquP9ZyLYD3jASAM0R-wcBRuHdWg10bUguH2bo_u64Z0mRKkIOrzILlHQ4ldmT0HirQIg8.png?r=bf0</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>스티븐 퀘일</t>
+          <t>짐 자무시</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>니콜라스 디아고스토,엠마 벨,마일스 피셔,엘런 로,재클린 매키니스 우드,P.J. 번,아를렝 이스카르페타,데이비드 코에너,코트니 B. 밴스,토니 토드</t>
+          <t>틸다 스윈튼,톰 히들스턴,미아 와시코우스카,존 허트,안톤 옐친,제프리 라이트,슬리만 다지</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>에릭 하이저러</t>
+          <t>짐 자무시</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>미국 영화,영화·호러,피투성이 호러 영화,영화·호러·초자연</t>
+          <t>영국 영화,드라마 장르 영화,드라마 장르 영화·로맨스,영화·로맨스</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>무서운,폭력</t>
+          <t>등골 서늘,색다른 이야기</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/E8vDc_W8CLv7-yMQu8KMEC7Rrr8/AAAABbqPXNSjI1U8tZIfZJ-tiM3AitY7UBrZfHMj8oGeBmPpoTxe-loumFg7GW3WLQ-ZW3aMv_qxk29lWKIcbwO7FauoEmQHOk1TSA.jpg?r=639</t>
+          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/E8vDc_W8CLv7-yMQu8KMEC7Rrr8/AAAABSbEMNrusMOYdEer4y_BP-liLaMbFR3hy95ainwphkm6ydgv8kF2d45sB0YzvyoYClMnWtvBVJbAe-9ub0e9h5TNAc3YPQk9pQ.jpg?r=6e9</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>위자</t>
+          <t>로마 위드 러브</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>단짝 친구의 갑작스러운 죽음. 남은 친구들은 아직 그녀를 보낼 마음의 준비가 되지 않았는데. 결국 다 같이 모여 낡은 보드게임을 꺼낸다. 그리곤 죽은 그녀와 대화를 시도하는데. 하지만 그들이 불러낸 것은, 저세상에서 온 악몽.</t>
+          <t>우디 앨런이 감독한 이 오락 영화는 로맨스와 부정, 오페라, 유명인사의 변덕을 주제로 한 4개의 이야기로 구성된다.</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>1시간 29분</t>
+          <t>1시간 51분</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2014</t>
+          <t>2012</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>만 15세 이상의 자가 관람할 수 있는 영화</t>
+          <t>청소년은 관람할 수 없는 영화</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/jsgGe9NCko3c-j0wGZ7FSwVlHs0/AAAABTIPP6fp3K6msYclU8UgKKG0PfcHA0qIbmsnaANMmvlPTTQ4Z_2eIIPRTLZjEUZqkduw02bqA-7ucu7FOjlNuag_ciIU_0fswkabjmA.png?r=271</t>
+          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/jsgGe9NCko3c-j0wGZ7FSwVlHs0/AAAABSNINBwNqEult8Zx5PlTEMqO3IIZIZg7uFVsLhfjSHeoUeatz0k2R3-sb5SGrCOArXxxyohWOdt3MKaOyoAzxYxKPN4veUfvcaoyU2I.png?r=ca9</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>스타일스 화이트</t>
+          <t>우디 앨런</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>올리비아 쿡,아나 코토,대런 카가소프,비앙카 A. 샌토스,더글러스 스미스,셸리 헤니그,시에라 휴어먼,서니 메이 앨리슨,린 샤예,비비스 콜롬베티</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr"/>
+          <t>우디 앨런,알렉 볼드윈,로베르토 베니니,페넬로페 크루즈,주디 데이비스,제시 아이젠버그,그레타 거윅,엘런 페이지,알레산드로 티베리,알레산드라 마스트로나르디,파비오 아르밀리아토,알리슨 필,플라비오 파렌티</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>우디 앨런</t>
+        </is>
+      </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>미국 영화,영화·호러,영화·호러·초자연,비명 유발·10대</t>
+          <t>미국 영화,영화·로맨스,로맨틱 코미디,코미디</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>등골 서늘,서스펜스</t>
+          <t>위트,로맨스</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/E8vDc_W8CLv7-yMQu8KMEC7Rrr8/AAAABRYLuZcHn-ntPiCekLKrpPWMpOyWZ0IexZgbpd554OWrr9PAMdKio3pSKVeq2aTc1E065CjGhvCdqamNV7JrjlqTSep-Bo0S6Q.jpg?r=74a</t>
+          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/E8vDc_W8CLv7-yMQu8KMEC7Rrr8/AAAABVDKOUoLxkdWsWcnXqr5zQefjA2hq8KK4qjP7BmNd_CaeZ0OkTYahr6gQjrzCmt-MUoHcNArpfNTUPv5AZsTQWuQhIXP3C6PmA.jpg?r=c04</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>언프렌디드: 친구삭제</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>별생각 없이 인터넷에 올린 영상. 장난삼아 저지른 괴롭힘은 친구의 자살이라는 비극을 낳고, 그로부터 1년 후 온라인에서 잔혹한 복수극이 시작되는데. 누구도 안전할 수 없다. 정체를 알 수 없는 추격자의 손에서.</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>1시간 22분</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>2014</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>만 15세 이상의 자가 관람할 수 있는 영화</t>
-        </is>
-      </c>
+          <t>만킬로미터</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr">
         <is>
-          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/jsgGe9NCko3c-j0wGZ7FSwVlHs0/AAAABaBkH24h7hscrtc4C70TQJq-pLMEBJZ48T3HuJ42Qr0aSF6STnxnWLcmflY2kwFjrDzLXutT3gtltW7xAAQTFOdWpupqcuR54p6fVGk.png?r=1f6</t>
+          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/jsgGe9NCko3c-j0wGZ7FSwVlHs0/AAAABbvA1nQiNNxFgBbGuV3jC9lZbB2P8S_7AYXoDew7fXW4mTSwGsX67iSH47CHOFvqCONrT2IbEFsNqdGx-mXIPEvvlgM8WqgL1waBa_A.png?r=d2f</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>레반 가브리아제</t>
+          <t>카를로스 마르케스메르세트</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>셸리 헤니그,모지스 스톰,르네 올스테드,윌 펠츠,제이컵 와이소키,코트니 핼버슨,헤더 소서먼,매슈 보러,미키 리버,캘 반스</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>넬슨 그리브스</t>
-        </is>
-      </c>
+          <t>내털리 테나,데이비드 베르다게르</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr">
         <is>
-          <t>미국 영화,영화·호러,영화·호러·초자연,비명 유발·10대</t>
+          <t>스페인 영화,드라마 장르 영화,드라마 장르 영화·로맨스,드라마 장르 영화·관능적</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>무서운,어두운 분위기</t>
+          <t>관능적</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/E8vDc_W8CLv7-yMQu8KMEC7Rrr8/AAAABdmCWy2bqbGUMgsFx8s_hcfDrTLT9ewmm2Ts-KV_qDYvqoBPlPw9gniSv0KfEQrYTSYWJHYyBt3gs7jr99AbjxahzOYmLS9Rvw.jpg?r=b18</t>
+          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/E8vDc_W8CLv7-yMQu8KMEC7Rrr8/AAAABbDkw6Q4cMiNL1eMDQGCCd9zmR131w9_2dLgyOnXCIpR9aXG4OpOITm3jNAL_2pxUHcfVhXxcTT2iJjXulxQ9LkNpufWp7p0dg.jpg?r=092</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>샤이닝</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>잭 토런스는 비수기의 적막하고 으스스한 호텔에서 생활하며 서서히 광기에 빠져들게 되고, 부인과 어린 아들을 공포에 빠뜨린다.</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>1시간 59분</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>1980</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>청소년은 관람할 수 없는 영화</t>
-        </is>
-      </c>
+          <t>미스 리틀 선샤인</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr">
         <is>
-          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/jsgGe9NCko3c-j0wGZ7FSwVlHs0/AAAABS6fDH2WJT0MPbnbNUpx51MEReOTsA3yRL5KOf8h9BCeqFPlkSyVbjpA5o9Wl8DT2e2WOuNn8OaSPw3ci5MSKY53wnGMKHpvVado-rw.png?r=6a1</t>
+          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/jsgGe9NCko3c-j0wGZ7FSwVlHs0/AAAABRTWkQW0EceEHqfAPy6BZp1ijBGNKsB9G0iKaO3WWtufJpE_dxCjzqlIZD49dNRS-W9OQ8k8wkfcG918uskLl1Utb0c9CB9b6-xFPus.png?r=3f4</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>스탠리 큐브릭</t>
+          <t>조너선 데이턴,밸러리 패리스</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>잭 니콜슨,셜리 듀발,대니 로이드,스캣맨 크로더스,베리 넬슨,필립 스톤,조 터켈,앤 잭슨,토니 버톤,리아 벨덤</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>스탠리 큐브릭,다이앤 존슨</t>
-        </is>
-      </c>
+          <t>그레그 키니어,스티브 커렐,토니 콜렛,폴 다노,아비게일 브레스린,앨런 아킨,브라이언 크랜스톤,딘 노리스,월리스 랭엄,베스 그랜트</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr">
         <is>
-          <t>미국 영화,영화·도서 원작,스릴러,스릴러·초자연</t>
+          <t>미국 영화,코미디,블랙 코미디,인디 영화</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>무서운,서스펜스</t>
+          <t>엉뚱하고 기발</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/E8vDc_W8CLv7-yMQu8KMEC7Rrr8/AAAABVCcKSMEUdpfRDYkGMhXZfOdcc7vvAip7VzccfXKVciSfYp2LJGrgX8kb6q2kSaIpZcyyWDXHhNNLaP1hUaboeZU-i7rVT8W_Q.jpg?r=210</t>
+          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/E8vDc_W8CLv7-yMQu8KMEC7Rrr8/AAAABSAIGok7DIRJAKiZkpuwXQRVPioLgDpyTSCkYCiVq8rWkMETWGa46IGZwsibAHwOaKCsxba0dO7X5fuKX3mESJ_jdRJSmSGIQw.jpg?r=516</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>귀신온천여관</t>
+          <t>FYRE: 꿈의 축제에서 악몽의 사기극으로</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>고향 가는 전학생한테 따라붙은 왕따 학생 둘. 가족이 온천 여관을 한다기에 잔뜩 기대했더니, 무슨 여관이 귀신의 집 뺨칠 만큼 으스스하다. 식구들은 더 으스스하다. 때리는 애들 무서워서 도망 왔더니, 뭐야 여기가 훨씬 무섭잖아!</t>
+          <t>지상 최고의 음악 축제가 열린다! 기발하고 화려한 홍보로 기대를 모았던 파이어 페스티벌. 하지만 그림 같은 해변의 빌라도, 근사한 파티도, 모두 거짓에 불과했다.</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1시간 48분</t>
+          <t>1시간 37분</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2018</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>만 12세 이상의 자가 관람할 수 있는 영화</t>
+          <t>만 15세 이상의 자가 관람할 수 있는 영화</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/jsgGe9NCko3c-j0wGZ7FSwVlHs0/AAAABfH_jvWz0OLU8jIhY_t8JAhWauUyD2Uo5H5u2uyy1co7bMcbdCWmnhsuz4l9vWOOHdFfzMiTOgUd4d22R9jwtyl7m85LLTEGYQk6bX0.png?r=248</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>장팅후,훙옌샹,린허쉬안,곽서요,나가영,주미미</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr"/>
+          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/jsgGe9NCko3c-j0wGZ7FSwVlHs0/AAAABQs9MOJRmjbhDw-T155YoclFYPww3TqDrZYWKfTMwVc6fqyKws2RUZzFmbGjcy47fvU0hNVgNIbCQDBFwCJ0dOPyj6hNLCnu6X8s_4FBsRVhifbUr2nEpz-2cBghuv_FFQDhbG56Y1ndAS3i_x5vzY7zqeWiuMiWS8kfhlgzkZE.png?r=b34</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>크리스 스미스</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>크리스 스미스</t>
+        </is>
+      </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>십대 영화,대만 영화,중국 영화,영화·호러</t>
+          <t>미국 영화,다큐멘터리</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>푼수 캐릭터,서스펜스</t>
+          <t>도발</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/E8vDc_W8CLv7-yMQu8KMEC7Rrr8/AAAABTUWY9lFt_oAjl27EBfMWszNTUGzJenMTWXuH5EzLUSKxh8l-8X1UShZ4T4FpEyouP3ZLP6GY9dwVu-6jhdklqVGwYOWE4ElXw.jpg?r=5aa</t>
+          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/E8vDc_W8CLv7-yMQu8KMEC7Rrr8/AAAABRT3-s9LxDCJM2YqeucMopkPbpQ-OS3_A8cbgx14W22Va_W-Oa7jLYP7NKJKr6gy3U0Kesgk_lharx5XelxQ7821-ZO8z3WyCA.jpg?r=0f3</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>퍼펙션</t>
+          <t>대학살: 나치 강제수용소</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>천재 첼리스트였던 샬럿. 10년 만에 돌아오니 신예 연주가가 정상에 올라 있다. 새로운 스타를 향한 그녀의 감정은 질투일까, 음악적 갈구일까. 그게 무엇이든 서막에 불과할 뿐. 지축을 뒤흔들 샬럿의 도발이 시작된다.</t>
+          <t>해방 후 나치 강제수용소의 참상을 보여주는 충격적 영상. 아이젠하워 장군의 명령으로 부헨발트, 오어드루프 등지를 둘러보는 나치의 모습도 담았다.</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>1시간 30분</t>
+          <t>58분</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>1945</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1167,54 +1123,46 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/jsgGe9NCko3c-j0wGZ7FSwVlHs0/AAAABfIdd2V39by2aadxBtxb67BshxNlRv1K8OWtwEzw3On8CkmH_RNw084j3uY0-M1G8odz6XdOzqGTeiNmad9y0BRSFXLfEDGhZJAJpe5Sxls6jVAr_x7eY1wCEWYqKj4Kl2mUGr-XbrXXUWE0mcTsBkMbWLfS7VTGuX2oTyWMgu4.png?r=281</t>
+          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/jsgGe9NCko3c-j0wGZ7FSwVlHs0/AAAABQRhAADHEboj8ReNU2FVeL3NL9x-kTGOIKrZIgh0JULbfd8cgyo8LenysIe-mPtIvEotFx4It5y-doQyXarteRaRWGgODE6eGgNZVbY.png?r=bed</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>리처드 쉐퍼드</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>앨리슨 윌리엄스,로건 브라우닝,스티븐 웨버,엘레이나 허프먼,마크 캔드보그,그램 더피</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>리처드 쉐퍼드,에릭 C. 차멜로,니콜 스나이더</t>
-        </is>
-      </c>
+          <t>조지 스티븐스</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr">
         <is>
-          <t>LGBTQ 영화,미국 영화,스릴러,심리 스릴러</t>
+          <t>미국 영화,다큐멘터리,역사 다큐멘터리,고전 영화</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>서스펜스</t>
+          <t>도발</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/E8vDc_W8CLv7-yMQu8KMEC7Rrr8/AAAABTctcDOxydqZxgTvRPF0gEln8YaiP45fnjueEgkBHzQxogq1EdBXW1Pa96JbOWmCfaGJE7kJLBXarv8aUDqRobJ-UA19iD3beQ.jpg?r=c7e</t>
+          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/E8vDc_W8CLv7-yMQu8KMEC7Rrr8/AAAABWyEHZlaphrxA5fhbswuc1Z_IRwjont1MXpo8zYeZw2uZtAN53fY5dnqy0KjGSOpJi8EIX-FIoVK_HzyqpaoytkDdJuuONrZsg.jpg?r=c96</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>마더!</t>
+          <t>제로 베팅 게임</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>한 시인과 그의 아내가 살고 있는 조용한 외딴집. 어느 날 초대받지 않은 낯선 사람들이 들이닥치며 집의 평화는 깨지고 만다. 심지어 무례하고 거침없는 사람들. 손님들은 점차 광기를 드러내고, 집 안에선 이상한 일들이 이어진다.</t>
+          <t>다단계 판매로 비난을 받는 세계적 건강식품회사 허벌라이프의 복잡한 세계를 심층 취재한 다큐멘터리.</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2시간 1분</t>
+          <t>1시간 44분</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1224,54 +1172,50 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>청소년은 관람할 수 없는 영화</t>
+          <t>만 12세 이상의 자가 관람할 수 있는 영화</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/jsgGe9NCko3c-j0wGZ7FSwVlHs0/AAAABRxRcCpcxG6STMApwxZ227RWBpQGrleCUCJ6Zh3gN4V-P6Vsswj8j1P9iz4ozgG0n91jhoDBj-0cg7HgwsL85KA2TQxwQlqdwWaXc8E.png?r=337</t>
+          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/jsgGe9NCko3c-j0wGZ7FSwVlHs0/AAAABQshU9j-dqr_mAUWm9wcArpvntfJl43tRqsF060i7KMIifG9Xvw0WT1Nntrw0kla56HV-QkmLcVBJVDgF4v_x4tY493mXiEBOjSSBeY.png?r=b84</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>대런 아로노프스키</t>
+          <t>테드 브라운</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>제니퍼 로런스,하비에르 바르뎀,에드 해리스,미셸 파이퍼,브라이언 글리슨,돔놀 글리슨,크리스틴 위그,스티븐 맥허티</t>
+          <t>윌리엄 액크먼</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>대런 아로노프스키</t>
+          <t>테드 브라운</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>미국 영화,영화·호러</t>
-        </is>
-      </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>무서운,어두운 분위기</t>
-        </is>
-      </c>
+          <t>미국 영화,다큐멘터리</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr">
         <is>
-          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/E8vDc_W8CLv7-yMQu8KMEC7Rrr8/AAAABQWhdYyKjVrE7qHoBj9Cvw0MekpHWE3281YGeIU6z8O1aDVmLJYvFQgiyc8-7sm2nzCwAaaapmVZt3tVKXWXIKtHZkityYySuA.jpg?r=29d</t>
+          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/E8vDc_W8CLv7-yMQu8KMEC7Rrr8/AAAABZ5ZWaiYAsHhRlwd6Pyj9HGBGGFUZESEEkzRohYWPrv98mFQREShLGYN9cDruqEf7nUd07o6nQyuBJ48Yu6Uv1-Bkv9SwZdvTg.jpg?r=dea</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>비밀스러운 초대</t>
+          <t>휘트니 휴스턴: 그냥 나로 살고자</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>한 남자가 자신의 전 부인이 여는 디너 파티에 초대받아 참석한다. 파티는 해묵은 상처가 드러나고 새로운 긴장 관계가 조성되는 불안한 자리가 되고만다.</t>
+          <t>팝 역사의 한 페이지를 장식한 가수 휘트니 휴스턴. 가수 데뷔부터 약물 중독과의 사투, 그리고 충격적인 죽음까지 원조 디바가 남기고 간 삶의 자취를 따라가 본다.</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1281,64 +1225,56 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2015</t>
+          <t>2016</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>청소년은 관람할 수 없는 영화</t>
+          <t>만 15세 이상의 자가 관람할 수 있는 영화</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/jsgGe9NCko3c-j0wGZ7FSwVlHs0/AAAABa112Gfoc88DOVrf0xhVcZEkWIm9wi5kP5HQgfd6pR7hm3jiqXwVwI386IkbIU8vAqJz43gmOmuYNjUXIKvDqeno30-Bbx1s_UtcKrc.png?r=c3f</t>
+          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/jsgGe9NCko3c-j0wGZ7FSwVlHs0/AAAABR8Xgmsvyj_FKpVE5B5SbIXiP0ytGc-NSunnHCSNPBYUtwjj31brWpCBeAsTa3TuXl9p9Q6JwznO9ywv25rzkiwCfsy893hpPXEo8uI.png?r=3ef</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>캐린 쿠사마</t>
+          <t>닉 브룸필드</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>로건 마샬 그린,타미 브랜차드,에마야치 코리날디,에이든 러브캠프,미쉘 크루지엑,마이크 도일,조디 빌라수소,제이 라슨,마리에 델피노,미힐 하위스만,린지 버지,존 캐럴 린치</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>필 헤이,맷 만프레디</t>
-        </is>
-      </c>
+          <t>휘트니 휴스턴</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr">
         <is>
-          <t>미국 영화,스릴러,심리 스릴러,영화·호러</t>
-        </is>
-      </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>무서운,폭력</t>
-        </is>
-      </c>
+          <t>록 &amp; 팝 콘서트,전기 영화,미국 영화,다큐멘터리</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr">
         <is>
-          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/E8vDc_W8CLv7-yMQu8KMEC7Rrr8/AAAABVqQdRLsPJjlt2i6T86ORyfYQiBYHsHzqKIVxZcZ9BAf4A0D5ESjAXbMtyNOqK4rfsBR_b5OAv8Oj4jgkBu-SjOk2LqAYjfoIQ.jpg?r=b87</t>
+          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/E8vDc_W8CLv7-yMQu8KMEC7Rrr8/AAAABdkCjQeuacUQDZpUVxYuCpYxjPzBfZKv19z4l73EDZIJlqkN5G4P39PUVQTpD9aB_D4RIqnI4tizFbxtfb-4orpChV4B4XG_Kg.jpg?r=522</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>오만과 편견 그리고 좀비</t>
+          <t>아메리카 와일드</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>좀비로 들끓는 19세기 영국. 무술의 달인이 된 베넷 자매들이 치맛자락을 걷어붙이고 좀비와의 혈투에 나선다! 《오만과 편견》의 패러디 소설을 영화화한 작품.</t>
+          <t>경외감을 자아내는 자연경관, 길들여지지 않은 야생의 생명력. 태곳적 신비를 간직한 미국의 국립 공원들을 찾아가는 다큐멘터리. 배우 로버트 레드퍼드가 내레이션을 맡았다.</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1시간 47분</t>
+          <t>42분</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1348,224 +1284,200 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>만 15세 이상의 자가 관람할 수 있는 영화</t>
+          <t>모든 연령에 해당하는 자가 관람할 수 있는 영화</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/jsgGe9NCko3c-j0wGZ7FSwVlHs0/AAAABXiSDBVgnoIglc1NyMHcobVwUukOf1FI8snIsCMlnNgsJsxs1hN_bPi5caPLdDTFrBm-4KGwqBOSnKWtP2AvGZOWAWszkpX6qN_QPD0.png?r=c4f</t>
+          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/jsgGe9NCko3c-j0wGZ7FSwVlHs0/AAAABXN5x7domTTz5iITuqU7EWM-MyA5iOTqyDQRUD-QASRcof08flo1NTZFRm5EWbM9ZTbUP_yFTSYopfyRvtKXyHxKaPxB-8TwtZBHtGc.png?r=cdc</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>버 스티어스</t>
+          <t>그레그 맥길리브레이</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>릴리 제임스,샘 라일리,잭 휴스턴,벨라 헤스콧,엘리 뱀버,밀리 브래디,수키 워터하우스,더글러스 부스,샐리 필립스,찰스 댄스,레나 헤디,맷 스미스</t>
+          <t>로버트 레드퍼드</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>버 스티어스</t>
+          <t>스티븐 저드슨,티모시 카힐</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>영화·도서 원작,영국 영화,영화·호러,공포 코미디 영화</t>
+          <t>미국 영화,다큐멘터리,과학&amp;자연 다큐멘터리</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>위트,폭력</t>
+          <t>흥미진진</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/E8vDc_W8CLv7-yMQu8KMEC7Rrr8/AAAABe8twpXlVGpaAv6bsdgdpHpIX2jRyXx9NVLYZ64yaqcI4MouDqsMc4hr-87xX8T0w5lTy3JDEOFLFyFtAltRVAPhpP6cD9Rh0g.jpg?r=e55</t>
+          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/E8vDc_W8CLv7-yMQu8KMEC7Rrr8/AAAABc0T15YACXhe2mtR8hgH-y_M6dtIFChfCsAIPjQZdNT5y4FllzzfXqJEPrE04X13gfC6ydQf84k7uPXVPr4Po9a5kk1mY1KeLA.jpg?r=b09</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>범죄의 재구성</t>
+          <t>과학, 지식 릴레이</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>철옹성 한국은행이 뚫렸다! 모든 시스템을 속이고 거액과 함께 사라진 사기꾼들. 증거와 돈, 모든 것의 행방이 묘연하다. 목표는 하나였지만 서로 달랐던 그들의 속셈. 이제 목숨을 건 추격전이 시작된다. 이 판에선 누구도 믿지 마라.</t>
+          <t>인간은 자신을 둘러싼 거대한 세계를 얼마나 이해하고 있는가. 물리학에서 심리학까지, 다양한 분야의 과학자 9명이 인류의 가장 근원적인 물음을 던진다. 이 세상은 무엇으로 이루어져 있는가, 의식이란 무엇인가, 생명은 어디서 왔는가.</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1시간 55분</t>
+          <t>1시간 32분</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2004</t>
+          <t>2018</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>청소년은 관람할 수 없는 영화</t>
+          <t>모든 연령에 해당하는 자가 관람할 수 있는 영화</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/jsgGe9NCko3c-j0wGZ7FSwVlHs0/AAAABY0GAn4jkueOJuoglRjI_WDYMPg_j7C-32eqiWxVn3pwsuvLYk95gn-hC2eTQSYfrsKsXGh2JGhqV34xh0hthzE7fUmjZUscQsoE0VE.png?r=f6b</t>
+          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/jsgGe9NCko3c-j0wGZ7FSwVlHs0/AAAABXLw9Z8q6MkErsg1GePI6tGHVYmCzxSckcqDfrVQssysLFes9j1fX1S0QIiGTsji7vFXdZwIV5JSG26C4MRV5Lc3tpeNgeavtQvNJ2A.png?r=4e0</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>최동훈</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>박신양,염정아,백윤식,천호진,이문식,박원상,김상호,김윤석,유선</t>
-        </is>
-      </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>최동훈</t>
-        </is>
-      </c>
+          <t>이안 체니</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr">
         <is>
-          <t>한국 영화,액션 &amp; 어드벤처,액션·코미디,액션 &amp; 어드벤처·범죄</t>
-        </is>
-      </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>색다른 이야기,흥미진진</t>
-        </is>
-      </c>
+          <t>미국 영화,다큐멘터리,과학&amp;자연 다큐멘터리</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr">
         <is>
-          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/E8vDc_W8CLv7-yMQu8KMEC7Rrr8/AAAABX7N2np9CF3amMAaYtF0HxBw7BnRMyNW0o1sEIC_dFTFHCA_dc5ZBj6Sbg8i-SNG80js6fCEzwL6CBYniYkO3OS4j2zV2scecA.jpg?r=c05</t>
+          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/E8vDc_W8CLv7-yMQu8KMEC7Rrr8/AAAABfkIbvzCY3i43xTB_26RwzVYmW3iE8VE7vpq1aMEbO3TzhEwhgPIJfMP6O-0cs5Nd20Ek35Dh0iVxHkmlopSL8Vad6cI50b3HQ.jpg?r=276</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>나의 마더</t>
+          <t>하이클레어성의 비밀</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>지구에서 멸종된 인류. 소녀에겐 자신을 키워준 로봇 ‘마더’가 전부였고, 마더 역시 ‘딸’인 소녀가 전부였다. 그들은 안전했다. 낯선 인간 여자가 나타나기 전까진.</t>
+          <t>"다운튼 애비"의 배경으로 알려진 하이클레어성은 실제로 귀족들과 하인들의 집이었으며, 다채로운 역사를 가지고 있다.</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>1시간 53분</t>
+          <t>54분</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>2013</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>만 15세 이상의 자가 관람할 수 있는 영화</t>
+          <t>만 12세 이상의 자가 관람할 수 있는 영화</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/jsgGe9NCko3c-j0wGZ7FSwVlHs0/AAAABTfQhlyV00eQqsjAv_CfcJZKo3oSN_-GMBhfD-NU5Zy7dE1DD3LO-TTQbVssoH_ngKOzKqzK2s01MXoIfZdMLswhXsmXBktUWFzUCT4yKEDTeTyIjjrw_vZlx_o9EwGJnxq_U2Md6qBgXOc5rOhdyM2FKFR4WwzW2TLvpoYArR0.png?r=503</t>
+          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/jsgGe9NCko3c-j0wGZ7FSwVlHs0/AAAABel1ifTRo-T-bY2j8kz5ws3mduqTkof9Vx4q8TXYmj09heOHSPgZeh7PAhCTF6Gj235-6i8-HI-bF4V9XwT8OYMQUDAGn2V5F_iTEg8.png?r=ec7</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>그랜트 스푸토레</t>
+          <t>비키 매튜스</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>클라라 루고르,로즈 번,힐러리 스왱크,루크 호커</t>
-        </is>
-      </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>그랜트 스푸토레,마이클 로이드 그린</t>
-        </is>
-      </c>
+          <t>사무엘 웨스트</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr">
         <is>
-          <t>호주 영화,SF &amp; 판타지,사이버펑크,SF·스릴러</t>
-        </is>
-      </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>불길한 영화,서스펜스</t>
-        </is>
-      </c>
+          <t>영국 영화,다큐멘터리,다큐멘터리·사회 &amp; 문화</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr">
         <is>
-          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/E8vDc_W8CLv7-yMQu8KMEC7Rrr8/AAAABQEWNY9acBuoyBjaG1GlhBfYfjQW8UdITSqUcw2NpPuDS9daVZZDxLaN-8dmUfj0jkuUgkKhQNi4yzt_51Ci4dzwxJ1pRdyRRA.jpg?r=f36</t>
+          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/E8vDc_W8CLv7-yMQu8KMEC7Rrr8/AAAABbDUaIKzrvjc2nuzqYpUEzNbXPI3TQVBio0vPAu0D-o0TetnATD_qGWxNe69AbC5bbAb6s6s5HZhprIAC913GvloaeedTd-sBw.jpg?r=872</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>침묵</t>
+          <t>바다의 사냥꾼 자고</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>실패를 모르는 남자. 돈이 진심이라 믿는 남자. 그러나 젊은 약혼녀가 주검으로 발견되고 딸이 용의자로 몰리는 순간, 그가 알던 세상은 순식간에 사라졌다. 모든 걸 걸고 딸을 무죄로 만들어라. 그리하지 않으면 모든 걸 잃을 터이니.</t>
+          <t>80대 노인이 산소통도 없이 작살 하나만 들고 바닷속으로 뛰어든다. 심해 사냥이라는 인도네시아 바자우족의 놀라운 전통을 이어가는 노인의 이야기를 담은 다큐멘터리.</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2시간 5분</t>
+          <t>48분</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2017</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>만 15세 이상의 자가 관람할 수 있는 영화</t>
+          <t>모든 연령에 해당하는 자가 관람할 수 있는 영화</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/jsgGe9NCko3c-j0wGZ7FSwVlHs0/AAAABYID6lcWbdeElYJwbp4G89h-mYtkhnUmJ_l7zpzr20cVQ2a_nKFuz6LUbuEHExrwlvNdVaL0lla-yddDVaM5hiukuNh_sZAZLmwgIfg.png?r=75c</t>
+          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/jsgGe9NCko3c-j0wGZ7FSwVlHs0/AAAABQ9LkgZdYxRSylqJhDOt7Bzw61YzJYSVql2Qx6p2QTL8uxmSLaEQJtVqiPJ_d3aXc9P4GYTO4emLtiuwPl554LEJd2pHwcVpZAgpUUs.png?r=150</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>정지우</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>최민식,박신혜,이하늬,이수경,류준열,박해준,조한철</t>
-        </is>
-      </c>
-      <c r="I24" t="inlineStr"/>
+          <t>제임스 리드,제임스 모건</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>제임스 리드</t>
+        </is>
+      </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>한국 영화,미스터리,드라마 장르 영화,법정 영화·드라마 장르</t>
-        </is>
-      </c>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>어두운 분위기,서스펜스</t>
-        </is>
-      </c>
+          <t>영국 영화,다큐멘터리,과학&amp;자연 다큐멘터리,다큐멘터리·사회 &amp; 문화</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr"/>
       <c r="L24" t="inlineStr">
         <is>
-          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/E8vDc_W8CLv7-yMQu8KMEC7Rrr8/AAAABe0qw732_0GeHFc1bykVeyFO8tbBasoRzpaqPFYZkMOYt1Zmxguy6CrA0ICxLPevmlcWdkqW09EahAiiGESTHla11MXP1W4uYQ.jpg?r=61e</t>
+          <t>https://occ-0-2794-2219.1.nflxso.net/dnm/api/v6/E8vDc_W8CLv7-yMQu8KMEC7Rrr8/AAAABTgX___awZMswrcy1Zzztvc7KfaSH16wyG-3gVL9VdCW56bA3VHMK1jAIbPKuiP3luTn3SbGAeAkgxG5oyJ2Kd9SDGwLfJJNgg.jpg?r=4ad</t>
         </is>
       </c>
     </row>

</xml_diff>